<commit_message>
a whole lot of changes
Created new notebooks to account for impact of assignment grade

optimized according to R. Gonzalez and introduced some additional models

Insertyed new baseline makjority class approach
</commit_message>
<xml_diff>
--- a/Data/Modeling Stage/Feature Selection/Nova_IMS_feature_selection_Date_threshold_10.xlsx
+++ b/Data/Modeling Stage/Feature Selection/Nova_IMS_feature_selection_Date_threshold_10.xlsx
@@ -49,9 +49,6 @@
     <t>Feature</t>
   </si>
   <si>
-    <t>Days with no interaction</t>
-  </si>
-  <si>
     <t>Total time online (min)</t>
   </si>
   <si>
@@ -64,25 +61,28 @@
     <t>Clicks on course</t>
   </si>
   <si>
-    <t>Number of clicks</t>
-  </si>
-  <si>
     <t>Largest period of inactivity (h)</t>
   </si>
   <si>
     <t>Average session duration (min)</t>
   </si>
   <si>
+    <t>Days with no interaction (%)</t>
+  </si>
+  <si>
     <t>Resources viewed</t>
   </si>
   <si>
-    <t>Days with no interaction (%)</t>
+    <t>Days with no interaction</t>
+  </si>
+  <si>
+    <t>Number of clicks</t>
+  </si>
+  <si>
+    <t>Clicks on forum</t>
   </si>
   <si>
     <t>Start of Session 4 (%)</t>
-  </si>
-  <si>
-    <t>Clicks on forum</t>
   </si>
   <si>
     <t>Clicks per session</t>
@@ -91,7 +91,16 @@
     <t>Clicks per day</t>
   </si>
   <si>
+    <t>Number of sessions</t>
+  </si>
+  <si>
+    <t>Assignments viewed</t>
+  </si>
+  <si>
     <t>Links viewed</t>
+  </si>
+  <si>
+    <t>Average grade of assignments</t>
   </si>
   <si>
     <t>Start of Session 2 (%)</t>
@@ -103,37 +112,28 @@
     <t>Start of Session 5 (%)</t>
   </si>
   <si>
-    <t>Average grade of assignments</t>
+    <t>Clicks on folder</t>
   </si>
   <si>
-    <t>Number of sessions</t>
-  </si>
-  <si>
-    <t>Clicks on folder</t>
+    <t>Start of Session 9 (%)</t>
   </si>
   <si>
     <t>Start of Session 6 (%)</t>
   </si>
   <si>
-    <t>Assignments viewed</t>
-  </si>
-  <si>
-    <t>Start of Session 9 (%)</t>
+    <t>Start of Session 7 (%)</t>
   </si>
   <si>
     <t>Assignments submitted</t>
-  </si>
-  <si>
-    <t>Start of Session 7 (%)</t>
-  </si>
-  <si>
-    <t>Files downloaded</t>
   </si>
   <si>
     <t>Forum posts</t>
   </si>
   <si>
     <t>Number of days</t>
+  </si>
+  <si>
+    <t>Files downloaded</t>
   </si>
   <si>
     <t>Quizzes started</t>
@@ -683,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -701,7 +701,7 @@
         <v>1</v>
       </c>
       <c r="J6">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -744,10 +744,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -805,13 +805,13 @@
         <v>18</v>
       </c>
       <c r="B10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
       </c>
       <c r="D10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
@@ -837,13 +837,13 @@
         <v>19</v>
       </c>
       <c r="B11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
       </c>
       <c r="D11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
@@ -875,13 +875,13 @@
         <v>0</v>
       </c>
       <c r="D12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -893,7 +893,7 @@
         <v>1</v>
       </c>
       <c r="J12">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -901,19 +901,19 @@
         <v>21</v>
       </c>
       <c r="B13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -925,7 +925,7 @@
         <v>1</v>
       </c>
       <c r="J13">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -997,28 +997,28 @@
         <v>24</v>
       </c>
       <c r="B16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="b">
         <v>1</v>
       </c>
       <c r="F16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
       </c>
       <c r="I16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16">
         <v>5</v>
@@ -1029,31 +1029,31 @@
         <v>25</v>
       </c>
       <c r="B17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="b">
         <v>1</v>
       </c>
       <c r="I17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1064,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1093,13 +1093,13 @@
         <v>27</v>
       </c>
       <c r="B19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -1117,7 +1117,7 @@
         <v>1</v>
       </c>
       <c r="J19">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1125,28 +1125,28 @@
         <v>28</v>
       </c>
       <c r="B20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
       </c>
       <c r="D20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" t="b">
         <v>1</v>
       </c>
       <c r="I20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20">
         <v>4</v>
@@ -1157,28 +1157,28 @@
         <v>29</v>
       </c>
       <c r="B21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
       </c>
       <c r="D21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" t="b">
         <v>1</v>
       </c>
       <c r="I21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21">
         <v>4</v>
@@ -1189,10 +1189,10 @@
         <v>30</v>
       </c>
       <c r="B22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
@@ -1224,7 +1224,7 @@
         <v>0</v>
       </c>
       <c r="C23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
@@ -1245,7 +1245,7 @@
         <v>1</v>
       </c>
       <c r="J23">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1259,7 +1259,7 @@
         <v>0</v>
       </c>
       <c r="D24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -1277,7 +1277,7 @@
         <v>1</v>
       </c>
       <c r="J24">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1317,13 +1317,13 @@
         <v>34</v>
       </c>
       <c r="B26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
       </c>
       <c r="D26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -1352,10 +1352,10 @@
         <v>0</v>
       </c>
       <c r="C27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
@@ -1679,7 +1679,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -1711,7 +1711,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -1743,7 +1743,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -1807,7 +1807,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -1839,7 +1839,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -1871,7 +1871,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -1903,7 +1903,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -1935,13 +1935,13 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -1999,13 +1999,13 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
       </c>
       <c r="C12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -2026,12 +2026,12 @@
         <v>1</v>
       </c>
       <c r="J12">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -2063,10 +2063,10 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -2081,21 +2081,21 @@
         <v>1</v>
       </c>
       <c r="G14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
       </c>
       <c r="I14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -2130,28 +2130,28 @@
         <v>29</v>
       </c>
       <c r="B16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" t="b">
         <v>1</v>
       </c>
       <c r="F16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
       </c>
       <c r="I16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
         <v>5</v>
@@ -2159,7 +2159,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
@@ -2168,13 +2168,13 @@
         <v>0</v>
       </c>
       <c r="D17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="b">
         <v>1</v>
       </c>
       <c r="F17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -2191,7 +2191,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
@@ -2223,7 +2223,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B20" t="b">
         <v>0</v>
@@ -2290,7 +2290,7 @@
         <v>33</v>
       </c>
       <c r="B21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -2314,12 +2314,12 @@
         <v>1</v>
       </c>
       <c r="J21">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B22" t="b">
         <v>0</v>
@@ -2351,7 +2351,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B23" t="b">
         <v>0</v>
@@ -2383,7 +2383,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B24" t="b">
         <v>0</v>
@@ -2415,13 +2415,13 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" t="b">
         <v>0</v>
@@ -2433,13 +2433,13 @@
         <v>0</v>
       </c>
       <c r="G25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" t="b">
         <v>1</v>
       </c>
       <c r="I25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25">
         <v>3</v>
@@ -2447,7 +2447,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B26" t="b">
         <v>0</v>
@@ -2456,7 +2456,7 @@
         <v>0</v>
       </c>
       <c r="D26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -2465,21 +2465,21 @@
         <v>0</v>
       </c>
       <c r="G26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" t="b">
         <v>1</v>
       </c>
       <c r="I26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B27" t="b">
         <v>0</v>
@@ -2511,7 +2511,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
@@ -2543,13 +2543,13 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
@@ -2575,7 +2575,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
@@ -2584,7 +2584,7 @@
         <v>0</v>
       </c>
       <c r="D30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" t="b">
         <v>0</v>
@@ -2602,12 +2602,12 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B31" t="b">
         <v>0</v>
@@ -2639,7 +2639,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B32" t="b">
         <v>0</v>
@@ -2671,7 +2671,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>
@@ -2703,7 +2703,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B34" t="b">
         <v>0</v>
@@ -2735,7 +2735,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B35" t="b">
         <v>0</v>
@@ -2812,7 +2812,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -2876,7 +2876,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -2908,7 +2908,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -2940,7 +2940,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -2949,7 +2949,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -2967,7 +2967,7 @@
         <v>1</v>
       </c>
       <c r="J6">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2975,13 +2975,13 @@
         <v>19</v>
       </c>
       <c r="B7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
       </c>
       <c r="D7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -3004,7 +3004,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -3013,13 +3013,13 @@
         <v>1</v>
       </c>
       <c r="D8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
       </c>
       <c r="F8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -3036,7 +3036,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -3068,7 +3068,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -3132,10 +3132,10 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -3159,12 +3159,12 @@
         <v>1</v>
       </c>
       <c r="J12">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -3173,7 +3173,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
@@ -3182,24 +3182,24 @@
         <v>1</v>
       </c>
       <c r="G13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="b">
         <v>1</v>
       </c>
       <c r="I13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -3211,16 +3211,16 @@
         <v>1</v>
       </c>
       <c r="F14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
       </c>
       <c r="I14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <v>6</v>
@@ -3228,31 +3228,31 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
       </c>
       <c r="D15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="b">
         <v>1</v>
       </c>
       <c r="I15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
         <v>5</v>
@@ -3292,10 +3292,10 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -3304,19 +3304,19 @@
         <v>0</v>
       </c>
       <c r="E17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
       </c>
       <c r="G17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" t="b">
         <v>1</v>
       </c>
       <c r="I17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17">
         <v>5</v>
@@ -3324,31 +3324,31 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
       </c>
       <c r="D18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" t="b">
         <v>1</v>
       </c>
       <c r="I18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18">
         <v>5</v>
@@ -3356,31 +3356,31 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" t="b">
         <v>1</v>
       </c>
       <c r="F19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" t="b">
         <v>1</v>
       </c>
       <c r="I19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19">
         <v>5</v>
@@ -3388,7 +3388,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B20" t="b">
         <v>0</v>
@@ -3397,13 +3397,13 @@
         <v>1</v>
       </c>
       <c r="D20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
       </c>
       <c r="F20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
@@ -3420,7 +3420,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -3484,7 +3484,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B23" t="b">
         <v>0</v>
@@ -3516,7 +3516,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
@@ -3548,7 +3548,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" t="b">
         <v>0</v>
@@ -3580,16 +3580,16 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -3607,7 +3607,7 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -3644,7 +3644,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
@@ -3676,16 +3676,16 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B29" t="b">
         <v>0</v>
       </c>
       <c r="C29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -3708,13 +3708,13 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
       </c>
       <c r="C30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
@@ -3735,7 +3735,7 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -3772,7 +3772,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B32" t="b">
         <v>0</v>
@@ -3804,7 +3804,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>
@@ -3868,7 +3868,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B35" t="b">
         <v>0</v>
@@ -3945,7 +3945,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -3977,7 +3977,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -4009,7 +4009,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -4041,7 +4041,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -4050,13 +4050,13 @@
         <v>1</v>
       </c>
       <c r="D5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
       </c>
       <c r="F5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -4073,7 +4073,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -4105,7 +4105,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -4137,7 +4137,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -4169,16 +4169,16 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
       </c>
       <c r="C9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -4201,7 +4201,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -4216,7 +4216,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
@@ -4228,18 +4228,18 @@
         <v>1</v>
       </c>
       <c r="J10">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
       </c>
       <c r="C11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -4260,12 +4260,12 @@
         <v>1</v>
       </c>
       <c r="J11">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
@@ -4274,22 +4274,22 @@
         <v>1</v>
       </c>
       <c r="D12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
       </c>
       <c r="G12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="b">
         <v>1</v>
       </c>
       <c r="I12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12">
         <v>6</v>
@@ -4297,16 +4297,16 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
       </c>
       <c r="C13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
@@ -4315,13 +4315,13 @@
         <v>1</v>
       </c>
       <c r="G13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="b">
         <v>1</v>
       </c>
       <c r="I13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13">
         <v>6</v>
@@ -4329,7 +4329,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B14" t="b">
         <v>0</v>
@@ -4361,7 +4361,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -4393,13 +4393,13 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -4411,13 +4411,13 @@
         <v>1</v>
       </c>
       <c r="G16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
       </c>
       <c r="I16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16">
         <v>5</v>
@@ -4425,71 +4425,71 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
       </c>
       <c r="E17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
       </c>
       <c r="G17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" t="b">
         <v>1</v>
       </c>
       <c r="I17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
       </c>
       <c r="C18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
       </c>
       <c r="E18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" t="b">
         <v>1</v>
       </c>
       <c r="I18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B19" t="b">
         <v>0</v>
@@ -4521,31 +4521,31 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
       </c>
       <c r="D20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" t="b">
         <v>1</v>
       </c>
       <c r="I20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20">
         <v>4</v>
@@ -4553,7 +4553,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" t="b">
         <v>0</v>
@@ -4585,16 +4585,16 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
       </c>
       <c r="D22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -4617,7 +4617,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" t="b">
         <v>1</v>
@@ -4681,7 +4681,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B25" t="b">
         <v>0</v>
@@ -4713,7 +4713,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B26" t="b">
         <v>0</v>
@@ -4745,7 +4745,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B27" t="b">
         <v>0</v>
@@ -4777,7 +4777,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
@@ -4809,7 +4809,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B29" t="b">
         <v>0</v>
@@ -4841,7 +4841,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
@@ -4873,7 +4873,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B31" t="b">
         <v>0</v>
@@ -4905,7 +4905,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B32" t="b">
         <v>0</v>
@@ -4937,7 +4937,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>
@@ -4969,7 +4969,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B34" t="b">
         <v>0</v>
@@ -5001,7 +5001,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B35" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
almost done with 10% threshold
</commit_message>
<xml_diff>
--- a/Data/Modeling Stage/Feature Selection/Nova_IMS_feature_selection_Date_threshold_10.xlsx
+++ b/Data/Modeling Stage/Feature Selection/Nova_IMS_feature_selection_Date_threshold_10.xlsx
@@ -64,19 +64,22 @@
     <t>Clicks on course</t>
   </si>
   <si>
+    <t>Number of clicks</t>
+  </si>
+  <si>
     <t>Largest period of inactivity (h)</t>
   </si>
   <si>
     <t>Average session duration (min)</t>
   </si>
   <si>
+    <t>Days with no interaction (%)</t>
+  </si>
+  <si>
     <t>Resources viewed</t>
   </si>
   <si>
-    <t>Number of clicks</t>
-  </si>
-  <si>
-    <t>Days with no interaction (%)</t>
+    <t>Clicks on forum</t>
   </si>
   <si>
     <t>Clicks per session</t>
@@ -88,19 +91,7 @@
     <t>Number of sessions</t>
   </si>
   <si>
-    <t>Clicks on forum</t>
-  </si>
-  <si>
-    <t>Assignments viewed</t>
-  </si>
-  <si>
     <t>Links viewed</t>
-  </si>
-  <si>
-    <t>Start of Session 6 (%)</t>
-  </si>
-  <si>
-    <t>Start of Session 5 (%)</t>
   </si>
   <si>
     <t>Start of Session 2 (%)</t>
@@ -112,19 +103,31 @@
     <t>Start of Session 4 (%)</t>
   </si>
   <si>
+    <t>Start of Session 5 (%)</t>
+  </si>
+  <si>
     <t>Average grade of assignments</t>
+  </si>
+  <si>
+    <t>Clicks on folder</t>
+  </si>
+  <si>
+    <t>Start of Session 6 (%)</t>
+  </si>
+  <si>
+    <t>Assignments viewed</t>
   </si>
   <si>
     <t>Start of Session 9 (%)</t>
   </si>
   <si>
-    <t>Clicks on folder</t>
-  </si>
-  <si>
     <t>Assignments submitted</t>
   </si>
   <si>
-    <t>Quizzes started</t>
+    <t>Start of Session 7 (%)</t>
+  </si>
+  <si>
+    <t>Start of Session 8 (%)</t>
   </si>
   <si>
     <t>Files downloaded</t>
@@ -136,13 +139,10 @@
     <t>Number of days</t>
   </si>
   <si>
-    <t>Discussions viewed</t>
+    <t>Quizzes started</t>
   </si>
   <si>
-    <t>Start of Session 7 (%)</t>
-  </si>
-  <si>
-    <t>Start of Session 8 (%)</t>
+    <t>Discussions viewed</t>
   </si>
   <si>
     <t>Submissions (% of course total)</t>
@@ -805,13 +805,13 @@
         <v>18</v>
       </c>
       <c r="B10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
@@ -829,7 +829,7 @@
         <v>1</v>
       </c>
       <c r="J10">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -837,13 +837,13 @@
         <v>19</v>
       </c>
       <c r="B11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
@@ -861,7 +861,7 @@
         <v>1</v>
       </c>
       <c r="J11">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -875,25 +875,25 @@
         <v>1</v>
       </c>
       <c r="D12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="b">
         <v>1</v>
       </c>
       <c r="I12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -933,28 +933,28 @@
         <v>22</v>
       </c>
       <c r="B14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
       </c>
       <c r="F14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
       </c>
       <c r="I14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <v>5</v>
@@ -965,7 +965,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -974,7 +974,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -997,31 +997,31 @@
         <v>24</v>
       </c>
       <c r="B16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
       </c>
       <c r="I16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1032,7 +1032,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -1053,7 +1053,7 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1064,28 +1064,28 @@
         <v>1</v>
       </c>
       <c r="C18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
       </c>
       <c r="E18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" t="b">
         <v>1</v>
       </c>
       <c r="I18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1093,7 +1093,7 @@
         <v>27</v>
       </c>
       <c r="B19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -1102,10 +1102,10 @@
         <v>0</v>
       </c>
       <c r="E19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" t="b">
         <v>1</v>
@@ -1117,7 +1117,7 @@
         <v>1</v>
       </c>
       <c r="J19">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1128,28 +1128,28 @@
         <v>1</v>
       </c>
       <c r="C20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
       </c>
       <c r="E20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" t="b">
         <v>1</v>
       </c>
       <c r="I20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1157,28 +1157,28 @@
         <v>29</v>
       </c>
       <c r="B21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
       </c>
       <c r="D21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" t="b">
         <v>1</v>
       </c>
       <c r="I21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21">
         <v>4</v>
@@ -1192,7 +1192,7 @@
         <v>0</v>
       </c>
       <c r="C22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
@@ -1201,7 +1201,7 @@
         <v>0</v>
       </c>
       <c r="F22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22" t="b">
         <v>1</v>
@@ -1224,10 +1224,10 @@
         <v>0</v>
       </c>
       <c r="C23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -1259,7 +1259,7 @@
         <v>0</v>
       </c>
       <c r="D24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -1277,7 +1277,7 @@
         <v>1</v>
       </c>
       <c r="J24">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1349,7 +1349,7 @@
         <v>35</v>
       </c>
       <c r="B27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -1373,7 +1373,7 @@
         <v>0</v>
       </c>
       <c r="J27">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1384,7 +1384,7 @@
         <v>0</v>
       </c>
       <c r="C28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
@@ -1405,7 +1405,7 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1810,10 +1810,10 @@
         <v>10</v>
       </c>
       <c r="B6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -1839,7 +1839,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -1871,7 +1871,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -1903,7 +1903,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -1935,7 +1935,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -1999,13 +1999,13 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
       </c>
       <c r="C12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -2017,27 +2017,27 @@
         <v>1</v>
       </c>
       <c r="G12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" t="b">
         <v>1</v>
       </c>
       <c r="I12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
       </c>
       <c r="C13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -2049,16 +2049,16 @@
         <v>1</v>
       </c>
       <c r="G13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="b">
         <v>1</v>
       </c>
       <c r="I13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -2069,13 +2069,13 @@
         <v>0</v>
       </c>
       <c r="C14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
       </c>
       <c r="E14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -2095,31 +2095,31 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
       </c>
       <c r="C15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="b">
         <v>1</v>
       </c>
       <c r="I15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
         <v>5</v>
@@ -2127,13 +2127,13 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -2145,13 +2145,13 @@
         <v>1</v>
       </c>
       <c r="G16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
       </c>
       <c r="I16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16">
         <v>5</v>
@@ -2159,31 +2159,31 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="b">
         <v>1</v>
       </c>
       <c r="F17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" t="b">
         <v>1</v>
       </c>
       <c r="I17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17">
         <v>5</v>
@@ -2191,31 +2191,31 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
       </c>
       <c r="C18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
       </c>
       <c r="E18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>
       </c>
       <c r="G18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" t="b">
         <v>1</v>
       </c>
       <c r="I18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18">
         <v>5</v>
@@ -2223,34 +2223,34 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" t="b">
         <v>1</v>
       </c>
       <c r="I19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -2267,19 +2267,19 @@
         <v>0</v>
       </c>
       <c r="E20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" t="b">
         <v>1</v>
       </c>
       <c r="I20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20">
         <v>4</v>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B21" t="b">
         <v>0</v>
@@ -2296,7 +2296,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -2314,12 +2314,12 @@
         <v>1</v>
       </c>
       <c r="J21">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B22" t="b">
         <v>0</v>
@@ -2351,7 +2351,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B23" t="b">
         <v>0</v>
@@ -2383,7 +2383,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B24" t="b">
         <v>0</v>
@@ -2415,7 +2415,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B25" t="b">
         <v>0</v>
@@ -2447,16 +2447,16 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
       </c>
       <c r="D26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B27" t="b">
         <v>0</v>
@@ -2511,7 +2511,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
@@ -2543,16 +2543,16 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
       </c>
       <c r="D29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -2575,7 +2575,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
@@ -2639,7 +2639,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B32" t="b">
         <v>0</v>
@@ -2671,7 +2671,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>
@@ -2703,7 +2703,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" t="b">
         <v>0</v>
@@ -2735,7 +2735,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B35" t="b">
         <v>0</v>
@@ -2812,7 +2812,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -2844,7 +2844,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -2876,7 +2876,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -2908,7 +2908,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -2940,7 +2940,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -2949,7 +2949,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -2967,21 +2967,21 @@
         <v>1</v>
       </c>
       <c r="J6">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
       </c>
       <c r="D7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -3004,7 +3004,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -3068,7 +3068,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -3100,7 +3100,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -3132,10 +3132,10 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -3159,12 +3159,12 @@
         <v>1</v>
       </c>
       <c r="J12">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -3196,7 +3196,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -3260,7 +3260,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B16" t="b">
         <v>0</v>
@@ -3292,7 +3292,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -3324,7 +3324,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B18" t="b">
         <v>0</v>
@@ -3356,7 +3356,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -3388,7 +3388,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
@@ -3420,7 +3420,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B21" t="b">
         <v>0</v>
@@ -3484,7 +3484,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B23" t="b">
         <v>0</v>
@@ -3516,7 +3516,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
@@ -3548,7 +3548,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
@@ -3580,7 +3580,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B26" t="b">
         <v>0</v>
@@ -3612,7 +3612,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B27" t="b">
         <v>0</v>
@@ -3676,7 +3676,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B29" t="b">
         <v>0</v>
@@ -3708,7 +3708,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
@@ -3740,7 +3740,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B31" t="b">
         <v>0</v>
@@ -3772,7 +3772,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B32" t="b">
         <v>0</v>
@@ -3804,7 +3804,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>
@@ -3868,7 +3868,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B35" t="b">
         <v>0</v>
@@ -3977,7 +3977,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -4041,7 +4041,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -4073,7 +4073,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -4105,7 +4105,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -4114,13 +4114,13 @@
         <v>1</v>
       </c>
       <c r="D7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
       </c>
       <c r="F7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -4137,16 +4137,16 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -4175,7 +4175,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
@@ -4196,27 +4196,27 @@
         <v>1</v>
       </c>
       <c r="J9">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
       </c>
       <c r="C10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
       </c>
       <c r="F10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
@@ -4228,18 +4228,18 @@
         <v>1</v>
       </c>
       <c r="J10">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
       </c>
       <c r="C11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
@@ -4248,16 +4248,16 @@
         <v>1</v>
       </c>
       <c r="F11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" t="b">
         <v>1</v>
       </c>
       <c r="I11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <v>6</v>
@@ -4265,7 +4265,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
@@ -4274,13 +4274,13 @@
         <v>0</v>
       </c>
       <c r="D12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="b">
         <v>1</v>
       </c>
       <c r="F12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -4297,16 +4297,16 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
       </c>
       <c r="D13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
@@ -4329,16 +4329,16 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
       </c>
       <c r="C14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
@@ -4347,13 +4347,13 @@
         <v>1</v>
       </c>
       <c r="G14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
       </c>
       <c r="I14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <v>6</v>
@@ -4361,7 +4361,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -4393,7 +4393,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -4425,7 +4425,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -4457,13 +4457,13 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
@@ -4472,7 +4472,7 @@
         <v>0</v>
       </c>
       <c r="F18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
@@ -4484,21 +4484,21 @@
         <v>1</v>
       </c>
       <c r="J18">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
       </c>
       <c r="D19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -4521,7 +4521,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B20" t="b">
         <v>0</v>
@@ -4530,13 +4530,13 @@
         <v>0</v>
       </c>
       <c r="D20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
       </c>
       <c r="F20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
@@ -4553,7 +4553,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -4565,19 +4565,19 @@
         <v>0</v>
       </c>
       <c r="E21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" t="b">
         <v>1</v>
       </c>
       <c r="I21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21">
         <v>4</v>
@@ -4585,7 +4585,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" t="b">
         <v>0</v>
@@ -4617,7 +4617,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B23" t="b">
         <v>0</v>
@@ -4649,7 +4649,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B24" t="b">
         <v>0</v>
@@ -4681,7 +4681,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B25" t="b">
         <v>0</v>
@@ -4690,7 +4690,7 @@
         <v>0</v>
       </c>
       <c r="D25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
@@ -4699,21 +4699,21 @@
         <v>0</v>
       </c>
       <c r="G25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" t="b">
         <v>1</v>
       </c>
       <c r="I25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B26" t="b">
         <v>0</v>
@@ -4777,7 +4777,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
@@ -4786,13 +4786,13 @@
         <v>0</v>
       </c>
       <c r="D28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
       </c>
       <c r="F28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" t="b">
         <v>0</v>
@@ -4809,7 +4809,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B29" t="b">
         <v>0</v>
@@ -4841,7 +4841,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
@@ -4873,7 +4873,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B31" t="b">
         <v>0</v>
@@ -4905,7 +4905,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B32" t="b">
         <v>0</v>
@@ -4937,7 +4937,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>
@@ -4969,7 +4969,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B34" t="b">
         <v>0</v>
@@ -5001,7 +5001,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B35" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Corrected Scaling and Sampling
Both scaling and oversampling (when applicable) are now applied after the train val split
</commit_message>
<xml_diff>
--- a/Data/Modeling Stage/Feature Selection/Nova_IMS_feature_selection_Date_threshold_10.xlsx
+++ b/Data/Modeling Stage/Feature Selection/Nova_IMS_feature_selection_Date_threshold_10.xlsx
@@ -49,19 +49,19 @@
     <t>Feature</t>
   </si>
   <si>
-    <t>Days with no interaction</t>
-  </si>
-  <si>
     <t>Total time online (min)</t>
   </si>
   <si>
     <t>Start of Session 1 (%)</t>
   </si>
   <si>
-    <t>Clicks (% of course total)</t>
+    <t>Days with no interaction</t>
   </si>
   <si>
     <t>Clicks on course</t>
+  </si>
+  <si>
+    <t>Clicks (% of course total)</t>
   </si>
   <si>
     <t>Number of clicks</t>
@@ -73,37 +73,43 @@
     <t>Average session duration (min)</t>
   </si>
   <si>
+    <t>Resources viewed</t>
+  </si>
+  <si>
     <t>Days with no interaction (%)</t>
   </si>
   <si>
-    <t>Resources viewed</t>
+    <t>Clicks per day</t>
   </si>
   <si>
     <t>Clicks on forum</t>
   </si>
   <si>
+    <t>Start of Session 5 (%)</t>
+  </si>
+  <si>
     <t>Clicks per session</t>
   </si>
   <si>
-    <t>Clicks per day</t>
+    <t>Start of Session 4 (%)</t>
+  </si>
+  <si>
+    <t>Start of Session 2 (%)</t>
   </si>
   <si>
     <t>Number of sessions</t>
   </si>
   <si>
+    <t>Assignments viewed</t>
+  </si>
+  <si>
     <t>Links viewed</t>
   </si>
   <si>
-    <t>Start of Session 2 (%)</t>
+    <t>Start of Session 6 (%)</t>
   </si>
   <si>
     <t>Start of Session 3 (%)</t>
-  </si>
-  <si>
-    <t>Start of Session 4 (%)</t>
-  </si>
-  <si>
-    <t>Start of Session 5 (%)</t>
   </si>
   <si>
     <t>Average grade of assignments</t>
@@ -112,22 +118,19 @@
     <t>Clicks on folder</t>
   </si>
   <si>
-    <t>Start of Session 6 (%)</t>
-  </si>
-  <si>
-    <t>Assignments viewed</t>
-  </si>
-  <si>
     <t>Start of Session 9 (%)</t>
   </si>
   <si>
     <t>Assignments submitted</t>
   </si>
   <si>
-    <t>Start of Session 7 (%)</t>
+    <t>Start of Session 10 (%)</t>
   </si>
   <si>
-    <t>Start of Session 8 (%)</t>
+    <t>Discussions viewed</t>
+  </si>
+  <si>
+    <t>Quizzes started</t>
   </si>
   <si>
     <t>Files downloaded</t>
@@ -139,16 +142,13 @@
     <t>Number of days</t>
   </si>
   <si>
-    <t>Quizzes started</t>
+    <t>Start of Session 8 (%)</t>
   </si>
   <si>
-    <t>Discussions viewed</t>
+    <t>Start of Session 7 (%)</t>
   </si>
   <si>
     <t>Submissions (% of course total)</t>
-  </si>
-  <si>
-    <t>Start of Session 10 (%)</t>
   </si>
 </sst>
 </file>
@@ -805,13 +805,13 @@
         <v>18</v>
       </c>
       <c r="B10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
       </c>
       <c r="D10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
@@ -837,13 +837,13 @@
         <v>19</v>
       </c>
       <c r="B11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
@@ -861,7 +861,7 @@
         <v>1</v>
       </c>
       <c r="J11">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -875,25 +875,25 @@
         <v>1</v>
       </c>
       <c r="D12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" t="b">
         <v>1</v>
       </c>
       <c r="I12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -904,25 +904,25 @@
         <v>1</v>
       </c>
       <c r="C13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="b">
         <v>1</v>
       </c>
       <c r="I13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13">
         <v>5</v>
@@ -942,19 +942,19 @@
         <v>0</v>
       </c>
       <c r="E14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
       </c>
       <c r="I14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <v>5</v>
@@ -965,28 +965,28 @@
         <v>23</v>
       </c>
       <c r="B15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="b">
         <v>1</v>
       </c>
       <c r="F15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" t="b">
         <v>1</v>
       </c>
       <c r="I15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <v>5</v>
@@ -997,10 +997,10 @@
         <v>24</v>
       </c>
       <c r="B16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -1012,13 +1012,13 @@
         <v>1</v>
       </c>
       <c r="G16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
       </c>
       <c r="I16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16">
         <v>5</v>
@@ -1061,28 +1061,28 @@
         <v>26</v>
       </c>
       <c r="B18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" t="b">
         <v>1</v>
       </c>
       <c r="F18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" t="b">
         <v>1</v>
       </c>
       <c r="I18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18">
         <v>5</v>
@@ -1099,13 +1099,13 @@
         <v>0</v>
       </c>
       <c r="D19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" t="b">
         <v>1</v>
@@ -1117,7 +1117,7 @@
         <v>1</v>
       </c>
       <c r="J19">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1128,28 +1128,28 @@
         <v>1</v>
       </c>
       <c r="C20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
       </c>
       <c r="E20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" t="b">
         <v>1</v>
       </c>
       <c r="I20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1157,13 +1157,13 @@
         <v>29</v>
       </c>
       <c r="B21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
       </c>
       <c r="D21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -1189,28 +1189,28 @@
         <v>30</v>
       </c>
       <c r="B22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
       </c>
       <c r="E22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" t="b">
         <v>1</v>
       </c>
       <c r="I22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22">
         <v>4</v>
@@ -1224,10 +1224,10 @@
         <v>0</v>
       </c>
       <c r="C23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -1259,7 +1259,7 @@
         <v>0</v>
       </c>
       <c r="D24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -1277,7 +1277,7 @@
         <v>1</v>
       </c>
       <c r="J24">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1349,7 +1349,7 @@
         <v>35</v>
       </c>
       <c r="B27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -1373,7 +1373,7 @@
         <v>0</v>
       </c>
       <c r="J27">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1384,7 +1384,7 @@
         <v>0</v>
       </c>
       <c r="C28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
@@ -1405,7 +1405,7 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1679,7 +1679,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -1711,7 +1711,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -1743,7 +1743,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -1807,16 +1807,16 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
       </c>
       <c r="C6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -1839,7 +1839,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -1871,16 +1871,16 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
       </c>
       <c r="C8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -1909,10 +1909,10 @@
         <v>1</v>
       </c>
       <c r="C9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -1935,16 +1935,16 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
       </c>
       <c r="C10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -1999,13 +1999,13 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
       </c>
       <c r="C12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -2017,21 +2017,21 @@
         <v>1</v>
       </c>
       <c r="G12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="b">
         <v>1</v>
       </c>
       <c r="I12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -2063,31 +2063,31 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
       </c>
       <c r="F14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
       </c>
       <c r="I14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <v>5</v>
@@ -2095,10 +2095,10 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -2107,7 +2107,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -2127,22 +2127,22 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
       </c>
       <c r="D16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
@@ -2159,13 +2159,13 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -2177,13 +2177,13 @@
         <v>1</v>
       </c>
       <c r="G17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="b">
         <v>1</v>
       </c>
       <c r="I17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17">
         <v>5</v>
@@ -2191,31 +2191,31 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
       </c>
       <c r="C18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
       </c>
       <c r="E18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>
       </c>
       <c r="G18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" t="b">
         <v>1</v>
       </c>
       <c r="I18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18">
         <v>5</v>
@@ -2223,7 +2223,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B19" t="b">
         <v>0</v>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B21" t="b">
         <v>0</v>
@@ -2319,7 +2319,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B22" t="b">
         <v>0</v>
@@ -2351,7 +2351,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B23" t="b">
         <v>0</v>
@@ -2383,7 +2383,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B24" t="b">
         <v>0</v>
@@ -2415,7 +2415,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B25" t="b">
         <v>0</v>
@@ -2511,7 +2511,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
@@ -2543,7 +2543,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
@@ -2575,7 +2575,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
@@ -2639,7 +2639,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B32" t="b">
         <v>0</v>
@@ -2671,7 +2671,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>
@@ -2703,7 +2703,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B34" t="b">
         <v>0</v>
@@ -2735,7 +2735,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B35" t="b">
         <v>0</v>
@@ -2812,7 +2812,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -2940,7 +2940,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -2949,7 +2949,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -2967,21 +2967,21 @@
         <v>1</v>
       </c>
       <c r="J6">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
       </c>
       <c r="D7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -3004,7 +3004,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -3013,13 +3013,13 @@
         <v>1</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
       </c>
       <c r="F8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -3036,7 +3036,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -3068,7 +3068,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -3100,7 +3100,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -3132,10 +3132,10 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -3159,12 +3159,12 @@
         <v>1</v>
       </c>
       <c r="J12">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -3176,7 +3176,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
@@ -3191,12 +3191,12 @@
         <v>1</v>
       </c>
       <c r="J13">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -3228,22 +3228,22 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
       </c>
       <c r="D15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
@@ -3260,7 +3260,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B16" t="b">
         <v>0</v>
@@ -3272,7 +3272,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -3287,12 +3287,12 @@
         <v>1</v>
       </c>
       <c r="J16">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -3356,7 +3356,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -3388,10 +3388,10 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -3415,12 +3415,12 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B21" t="b">
         <v>0</v>
@@ -3429,7 +3429,7 @@
         <v>1</v>
       </c>
       <c r="D21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -3447,12 +3447,12 @@
         <v>1</v>
       </c>
       <c r="J21">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B22" t="b">
         <v>0</v>
@@ -3484,16 +3484,16 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B23" t="b">
         <v>0</v>
       </c>
       <c r="C23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -3516,7 +3516,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
@@ -3548,7 +3548,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
@@ -3580,16 +3580,16 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B26" t="b">
         <v>0</v>
       </c>
       <c r="C26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -3612,7 +3612,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" t="b">
         <v>0</v>
@@ -3682,10 +3682,10 @@
         <v>0</v>
       </c>
       <c r="C29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -3708,7 +3708,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
@@ -3740,7 +3740,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B31" t="b">
         <v>0</v>
@@ -3804,7 +3804,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>
@@ -3836,7 +3836,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B34" t="b">
         <v>0</v>
@@ -3868,7 +3868,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B35" t="b">
         <v>0</v>
@@ -4041,7 +4041,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -4050,7 +4050,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -4068,12 +4068,12 @@
         <v>1</v>
       </c>
       <c r="J5">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -4082,13 +4082,13 @@
         <v>1</v>
       </c>
       <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
       </c>
       <c r="F6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -4105,7 +4105,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -4137,16 +4137,16 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
       </c>
       <c r="D8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -4169,13 +4169,13 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
       </c>
       <c r="C9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
@@ -4196,27 +4196,27 @@
         <v>1</v>
       </c>
       <c r="J9">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
       </c>
       <c r="C10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
       </c>
       <c r="F10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
@@ -4228,12 +4228,12 @@
         <v>1</v>
       </c>
       <c r="J10">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -4242,7 +4242,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
@@ -4251,27 +4251,27 @@
         <v>1</v>
       </c>
       <c r="G11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="b">
         <v>1</v>
       </c>
       <c r="I11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
       </c>
       <c r="C12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
@@ -4280,16 +4280,16 @@
         <v>1</v>
       </c>
       <c r="F12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" t="b">
         <v>1</v>
       </c>
       <c r="I12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12">
         <v>6</v>
@@ -4297,7 +4297,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -4329,7 +4329,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -4341,7 +4341,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="b">
         <v>1</v>
@@ -4356,36 +4356,36 @@
         <v>1</v>
       </c>
       <c r="J14">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" t="b">
         <v>1</v>
       </c>
       <c r="F15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="b">
         <v>1</v>
       </c>
       <c r="I15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
         <v>5</v>
@@ -4393,7 +4393,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -4425,7 +4425,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -4457,39 +4457,39 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
       </c>
       <c r="C18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
       </c>
       <c r="E18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" t="b">
         <v>1</v>
       </c>
       <c r="I18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B19" t="b">
         <v>0</v>
@@ -4521,10 +4521,10 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -4536,7 +4536,7 @@
         <v>0</v>
       </c>
       <c r="F20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
@@ -4553,16 +4553,16 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
       </c>
       <c r="D21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -4585,7 +4585,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B22" t="b">
         <v>0</v>
@@ -4617,16 +4617,16 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B23" t="b">
         <v>0</v>
       </c>
       <c r="C23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -4649,7 +4649,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B24" t="b">
         <v>0</v>
@@ -4681,7 +4681,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B25" t="b">
         <v>0</v>
@@ -4713,7 +4713,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B26" t="b">
         <v>0</v>
@@ -4722,13 +4722,13 @@
         <v>0</v>
       </c>
       <c r="D26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
       </c>
       <c r="F26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" t="b">
         <v>0</v>
@@ -4777,7 +4777,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
@@ -4786,13 +4786,13 @@
         <v>0</v>
       </c>
       <c r="D28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
       </c>
       <c r="F28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28" t="b">
         <v>0</v>
@@ -4809,7 +4809,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B29" t="b">
         <v>0</v>
@@ -4841,7 +4841,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
@@ -4873,7 +4873,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B31" t="b">
         <v>0</v>
@@ -4905,7 +4905,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" t="b">
         <v>0</v>
@@ -4937,7 +4937,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>
@@ -4969,7 +4969,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B34" t="b">
         <v>0</v>
@@ -5001,7 +5001,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B35" t="b">
         <v>0</v>

</xml_diff>